<commit_message>
export to excel the new functionality for boundary condition
</commit_message>
<xml_diff>
--- a/QuantLibXL2/Workbooks/BermudanSwaption.xlsx
+++ b/QuantLibXL2/Workbooks/BermudanSwaption.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t>today's date</t>
   </si>
@@ -207,18 +207,31 @@
   </si>
   <si>
     <t>trigger</t>
+  </si>
+  <si>
+    <t>calculator</t>
+  </si>
+  <si>
+    <t>exercise</t>
+  </si>
+  <si>
+    <t>probabilities</t>
+  </si>
+  <si>
+    <t>rates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.0000000_);_(* \(#,##0.0000000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -265,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -278,6 +291,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -581,7 +595,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:D39"/>
+  <dimension ref="B2:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -589,7 +603,7 @@
   <cols>
     <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
@@ -643,7 +657,7 @@
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C9" s="4">
+      <c r="C9" s="10">
         <v>4.8758250000000003E-2</v>
       </c>
     </row>
@@ -652,7 +666,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="e">
-        <f ca="1">_xll.qlSimpleQuote(B10,C9,,C8)</f>
+        <f ca="1">_xll.qlSimpleQuote(B10,C9,,,C8)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -799,7 +813,7 @@
         <v>#NAME?</v>
       </c>
       <c r="D26" s="1" t="e">
-        <f t="array" aca="1" ref="D26:D31" ca="1">_xll.qlTemp1(C26)</f>
+        <f t="array" aca="1" ref="D26:D31" ca="1">_xll.qlSwapFixedLegAccrualStartDates(C26)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -833,7 +847,7 @@
       <c r="B29" t="s">
         <v>29</v>
       </c>
-      <c r="C29" t="e">
+      <c r="C29" s="10" t="e">
         <f ca="1">_xll.qlVanillaSwapFairRate(C26,C28)</f>
         <v>#NAME?</v>
       </c>
@@ -846,7 +860,7 @@
       <c r="B30" t="s">
         <v>30</v>
       </c>
-      <c r="C30" t="e">
+      <c r="C30" s="10" t="e">
         <f ca="1">C29*1.2</f>
         <v>#NAME?</v>
       </c>
@@ -859,7 +873,7 @@
       <c r="B31" t="s">
         <v>31</v>
       </c>
-      <c r="C31" t="e">
+      <c r="C31" s="10" t="e">
         <f ca="1">C30*0.8</f>
         <v>#NAME?</v>
       </c>
@@ -877,7 +891,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>33</v>
       </c>
@@ -886,7 +900,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>34</v>
       </c>
@@ -894,8 +908,17 @@
         <f ca="1">_xll.qlVanillaSwap(B34,C18,1000,C24,C31,C16,C25,C20,0,C21)</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>55</v>
       </c>
@@ -903,8 +926,17 @@
         <f ca="1">_xll.qlBermudanExercise(B35,D26:D30)</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>47</v>
       </c>
@@ -912,31 +944,114 @@
         <f ca="1">_xll.qlSwaption(,C32,C35)</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="e">
+        <f t="array" aca="1" ref="D36:D41" ca="1">_xll.qlSwaptionExerciseDates(C36,C40)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E36" s="10" t="e">
+        <f t="array" aca="1" ref="E36:E41" ca="1">_xll.qlSwaptionExerciseProbabilities(C36,C40)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F36" s="10" t="e">
+        <f t="array" aca="1" ref="F36:F41" ca="1">_xll.qlSwaptionExerciseRates(C36,C40)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" t="e">
+        <f ca="1">_xll.qlTreeCumulativeProbabilityCalculator1D()</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D37" s="1" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="E37" s="10" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="F37" s="10" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>59</v>
       </c>
-      <c r="C37" t="e">
-        <f ca="1">_xll.qlTreeSwaptionEngine(,Calibration_HW!B1,50,,Calibration_HW!B4)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="C38" t="e">
+        <f ca="1">_xll.qlTreeSwaptionEngine(,Calibration_HW!B1,50,,C37,,Calibration_HW!B4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D38" s="1" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="E38" s="10" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="F38" s="10" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>60</v>
       </c>
-      <c r="C38" t="e">
-        <f ca="1">_xll.qlInstrumentSetPricingEngine(C36,C37)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="C39" t="e">
+        <f ca="1">_xll.qlInstrumentSetPricingEngine(C36,C38)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D39" s="1" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="E39" s="10" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="F39" s="10" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="9" t="e">
-        <f ca="1">_xll.qlInstrumentNPV(C36,C38)</f>
+      <c r="C40" s="9" t="e">
+        <f ca="1">_xll.qlInstrumentNPV(C36,C39)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D40" s="1" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="E40" s="10" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="F40" s="10" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D41" s="1" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="E41" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="F41" t="e">
+        <f ca="1"/>
         <v>#NAME?</v>
       </c>
     </row>
@@ -952,7 +1067,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>